<commit_message>
Kosten angepasst und board config auf Arduino Mega geändert
</commit_message>
<xml_diff>
--- a/doc/Kosten.xlsx
+++ b/doc/Kosten.xlsx
@@ -5,20 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\PlatformIO\Projects\BudeRFID\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\BudeRFID\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8664B2D6-0F72-44D1-B0AC-A2E291A3E070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890217A1-70F7-4E1D-BB34-FB02D5886B9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B73F06C9-AE1E-46B2-ADCB-966F33681F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Arduino Uno</t>
-  </si>
-  <si>
     <t>Powerbank</t>
   </si>
   <si>
@@ -70,6 +76,9 @@
   </si>
   <si>
     <t>LCD 16x2 I2C (vorverlötet)</t>
+  </si>
+  <si>
+    <t>Arduino Mega</t>
   </si>
 </sst>
 </file>
@@ -439,7 +448,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,21 +459,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
-        <v>10.99</v>
+        <v>11.99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2">
         <v>14.24</v>
@@ -472,7 +481,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>4.99</v>
@@ -480,7 +489,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>6.29</v>
@@ -488,7 +497,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2">
         <v>2.99</v>
@@ -496,7 +505,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>3.99</v>
@@ -504,7 +513,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2">
         <v>3.61</v>
@@ -512,7 +521,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2">
         <v>5.95</v>
@@ -520,7 +529,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2">
         <v>6.99</v>
@@ -528,7 +537,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2">
         <v>5.85</v>
@@ -536,7 +545,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>4.9000000000000004</v>
@@ -544,7 +553,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>5.34</v>
@@ -552,19 +561,19 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="5">
         <f>SUM(B2:B14)</f>
-        <v>86.13000000000001</v>
+        <v>92.13000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kosten für Gehäuseherstellung ergänzt
</commit_message>
<xml_diff>
--- a/doc/Kosten.xlsx
+++ b/doc/Kosten.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\BudeRFID\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\BudeRFID\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890217A1-70F7-4E1D-BB34-FB02D5886B9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB12828E-B236-4E9E-BC58-07853C8371A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B73F06C9-AE1E-46B2-ADCB-966F33681F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Powerbank</t>
   </si>
@@ -66,19 +57,43 @@
     <t>Pauschale für Kabel und weiteres Zubehör</t>
   </si>
   <si>
-    <t>Summe</t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
-    <t>Kostenliste - BudeRFID</t>
-  </si>
-  <si>
     <t>LCD 16x2 I2C (vorverlötet)</t>
   </si>
   <si>
     <t>Arduino Mega</t>
+  </si>
+  <si>
+    <t>Preis pro kg</t>
+  </si>
+  <si>
+    <t>90° Adapter</t>
+  </si>
+  <si>
+    <t>USB Buchse</t>
+  </si>
+  <si>
+    <t>PLA Schwarz</t>
+  </si>
+  <si>
+    <t>PLA Transparent</t>
+  </si>
+  <si>
+    <t>Pauschale f. Gewinde etc.</t>
+  </si>
+  <si>
+    <t>Menge in kg</t>
+  </si>
+  <si>
+    <t>Preis in €</t>
+  </si>
+  <si>
+    <t>Bauteil</t>
+  </si>
+  <si>
+    <t>Gesamtkosten</t>
   </si>
 </sst>
 </file>
@@ -122,15 +137,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -445,135 +470,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6304C6CD-2E72-4481-897B-9A195114E46D}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="2"/>
+    <col min="2" max="2" width="10.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>11.99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>14.24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>4.99</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>6.29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>2.99</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>3.99</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>3.61</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>5.95</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>6.99</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5">
         <v>5.85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5">
         <v>5.34</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>10</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B16" s="5">
-        <f>SUM(B2:B14)</f>
-        <v>92.13000000000001</v>
+        <v>4.3899999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5">
+        <f>D18*C18</f>
+        <v>8.4208800000000004</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.312</v>
+      </c>
+      <c r="D18" s="7">
+        <v>26.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5">
+        <f>D19*C19</f>
+        <v>9.1038599999999992</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="D19" s="7">
+        <v>21.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="6">
+        <f>SUM(B2:B21)</f>
+        <v>125.34474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>